<commit_message>
batch fixing GPX files and imoport to single GPKG
</commit_message>
<xml_diff>
--- a/docs/formats/formats-and-transforms.xlsx
+++ b/docs/formats/formats-and-transforms.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/_WORK/map-projects/docs/formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDE4746-9E3C-0347-A339-4D28FD77C702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97354C2-C3F0-624E-B7C5-046CE01A62D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{BE81C301-35F6-7D49-8050-E301E34D041F}"/>
   </bookViews>
   <sheets>
     <sheet name="gpx" sheetId="1" r:id="rId1"/>
+    <sheet name="Fle Formats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t xml:space="preserve">how gpx elements are mapped to QGis and others </t>
   </si>
@@ -74,9 +75,6 @@
     <t>not used ?</t>
   </si>
   <si>
-    <t>qgis</t>
-  </si>
-  <si>
     <t>Google EarthPro</t>
   </si>
   <si>
@@ -119,9 +117,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>tracks.[*].name</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">imports as </t>
     </r>
@@ -222,13 +217,125 @@
       </rPr>
       <t xml:space="preserve"> for each continuous span of track data.</t>
     </r>
+  </si>
+  <si>
+    <t>ESRI Shapefile format</t>
+  </si>
+  <si>
+    <t>GeoPackage file</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">can contain </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>various data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (both </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vector and raster data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) in different coordinate reference systems, as well as tables
+without spatial information; all these features </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>allow you to share data easily and avoid file duplication</t>
+    </r>
+  </si>
+  <si>
+    <t>gpx/@version</t>
+  </si>
+  <si>
+    <t>strava</t>
+  </si>
+  <si>
+    <t>niekedy nie</t>
+  </si>
+  <si>
+    <t>qgis/gdal</t>
+  </si>
+  <si>
+    <t>WARNING ak neni vyplneny</t>
+  </si>
+  <si>
+    <t>trailforks</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>feature.name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Multipart to singlepart konverzia nastastie zachova name multiline na vsetkych single line</t>
+    </r>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>group name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -240,6 +347,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,10 +383,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -279,23 +395,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -608,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8909D83C-4036-AE48-BC90-C7A5A1198F41}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,158 +769,232 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
+      <c r="F3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="26" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>29</v>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:I1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{3E73D1B4-4031-1041-A5EB-3323235980FD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEAA4B8-0C18-5E4C-97B3-FBF456106612}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
handling emoty travk <name>
</commit_message>
<xml_diff>
--- a/docs/formats/formats-and-transforms.xlsx
+++ b/docs/formats/formats-and-transforms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/_WORK/map-projects/docs/formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97354C2-C3F0-624E-B7C5-046CE01A62D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1EC8B2-9B4B-E043-8CD6-AFAABF889FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{BE81C301-35F6-7D49-8050-E301E34D041F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t xml:space="preserve">how gpx elements are mapped to QGis and others </t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>group name</t>
+  </si>
+  <si>
+    <t>Source of data. Included to give user some idea of reliability and accuracy of data.</t>
+  </si>
+  <si>
+    <t>dal by sa naplnit z @gpx/creator</t>
   </si>
 </sst>
 </file>
@@ -413,26 +419,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -749,146 +755,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8909D83C-4036-AE48-BC90-C7A5A1198F41}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="43.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="60.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E2" s="7"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="5" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -896,69 +905,78 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{3E73D1B4-4031-1041-A5EB-3323235980FD}"/>

</xml_diff>

<commit_message>
Land Cover and PIA
</commit_message>
<xml_diff>
--- a/docs/formats/formats-and-transforms.xlsx
+++ b/docs/formats/formats-and-transforms.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/_WORK/map-projects/docs/formats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcus/workspaces/map-projects/docs/formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1EC8B2-9B4B-E043-8CD6-AFAABF889FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647CE4B2-8059-C745-BCE9-DBEFDACD6D85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{BE81C301-35F6-7D49-8050-E301E34D041F}"/>
+    <workbookView xWindow="10020" yWindow="1840" windowWidth="28040" windowHeight="16600" activeTab="2" xr2:uid="{BE81C301-35F6-7D49-8050-E301E34D041F}"/>
   </bookViews>
   <sheets>
     <sheet name="gpx" sheetId="1" r:id="rId1"/>
     <sheet name="Fle Formats" sheetId="2" r:id="rId2"/>
+    <sheet name="Glossary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t xml:space="preserve">how gpx elements are mapped to QGis and others </t>
   </si>
@@ -335,13 +336,221 @@
   </si>
   <si>
     <t>dal by sa naplnit z @gpx/creator</t>
+  </si>
+  <si>
+    <t>file extension</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Packages (ArcGis)</t>
+  </si>
+  <si>
+    <t>.lpk</t>
+  </si>
+  <si>
+    <t>Packages one or more layers and all referenced data sources to create a single compressed .lpk file.</t>
+  </si>
+  <si>
+    <t>WCS</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>WFS</t>
+  </si>
+  <si>
+    <t>WMS</t>
+  </si>
+  <si>
+    <t>WMST</t>
+  </si>
+  <si>
+    <t>webservices</t>
+  </si>
+  <si>
+    <t>https://www.ogc.org/standards/wmts</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Web Map Tile Service</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>raster</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Open Geospatial Consortium, Inc. (OGC) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Web Coverage Service (WCS) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">provides an open specification for sharing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>raster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> datasets on the web. 
+A WCS service returns data in a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>format that can be used as input for analysis and modeling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. This is in contrast with the OGC Web Map Service (WMS), which only returns a picture of the data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Web Feature Service (WFS) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Interface Standard provides an interface allowing requests for geographical features across the web using platform-independent calls.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Web Map Service,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Webová Mapová Služba (WMS) je štandardom vyvinutým a rozširovaným združením Open Geospatial Consortium (OGC). Služba pracuje na princípe klient-server a umožňuje zdieľanie priestorových údajov vo forme rastrových máp v prostredí Internetu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Web Map Tile Service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, A Web Map Tile Service (WMTS) is a standard protocol for serving pre-rendered or run-time computed georeferenced map tiles over the Internet. </t>
+    </r>
+  </si>
+  <si>
+    <t>Web Coverage Service</t>
+  </si>
+  <si>
+    <t>Abbrev</t>
+  </si>
+  <si>
+    <t>Web Feature Service</t>
+  </si>
+  <si>
+    <t>Web Map Service</t>
+  </si>
+  <si>
+    <t>vector
+raster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -361,6 +570,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -393,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -439,6 +655,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -757,7 +982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8909D83C-4036-AE48-BC90-C7A5A1198F41}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -987,32 +1212,171 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEAA4B8-0C18-5E4C-97B3-FBF456106612}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.5" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="78.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93CBA28-8264-4D4A-9230-DC135B00FC23}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="33.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{F69EB8E5-2829-2F43-B9B0-A8CEA093DACC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
extensions parsing, out formating, all in one algorithm
</commit_message>
<xml_diff>
--- a/docs/formats/formats-and-transforms.xlsx
+++ b/docs/formats/formats-and-transforms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcus/workspaces/map-projects/docs/formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647CE4B2-8059-C745-BCE9-DBEFDACD6D85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097C0AB0-365F-6847-A161-98D66938E137}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="1840" windowWidth="28040" windowHeight="16600" activeTab="2" xr2:uid="{BE81C301-35F6-7D49-8050-E301E34D041F}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16600" xr2:uid="{BE81C301-35F6-7D49-8050-E301E34D041F}"/>
   </bookViews>
   <sheets>
     <sheet name="gpx" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="110">
   <si>
     <t xml:space="preserve">how gpx elements are mapped to QGis and others </t>
   </si>
@@ -544,13 +544,260 @@
   <si>
     <t>vector
 raster</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Track Segment holds a list of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Track Points</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wptType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) which are logically connected in order. To represent a single GPS track where GPS reception was lost, or the GPS receiver was turned off, start a new Track Segment for each continuous span of track data.</t>
+    </r>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/ele</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/time</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/magvar</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/geoidheight</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/name</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/cmt</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/desc</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/src</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/link</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/sym</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/type</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/fix</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/sat</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/hdop</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/vdop</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/pdop</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/ageofdgpsdata</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/dgpsid</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/extensions</t>
+  </si>
+  <si>
+    <t>Magnetic variation (in degrees) at the point</t>
+  </si>
+  <si>
+    <r>
+      <t>Elevation (in meters) of the point. (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>nikde sa nepise v akej projekcii bvp vs….</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Creation/modification timestamp for element. Date and time in are in Univeral Coordinated Time (UTC), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">not local time! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Conforms to ISO 8601 specification for date/time representation. Fractional seconds are allowed for millisecond timing in tracklogs. </t>
+    </r>
+  </si>
+  <si>
+    <t>The GPS name of the waypoint. This field will be transferred to and from the GPS. GPX does not place restrictions on the length of this field or the characters contained in it. It is up to the receiving application to validate the field before sending it to the GPS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS waypoint comment. Sent to GPS as comment. </t>
+  </si>
+  <si>
+    <t>Source of data. Included to give user some idea of reliability and accuracy of data.  "Garmin eTrex", "USGS quad Boston North", e.g.</t>
+  </si>
+  <si>
+    <t>Link to additional information about the waypoint.</t>
+  </si>
+  <si>
+    <t>Text of GPS symbol name. For interchange with other programs, use the exact spelling of the symbol as displayed on the GPS.  If the GPS abbreviates words, spell them out.</t>
+  </si>
+  <si>
+    <t>Type (classification) of the waypoint.</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/extensions/gpxtpx:TrackPointExtension</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/extensions/gpxtpx:TrackPointExtension/gpxtpx:hr</t>
+  </si>
+  <si>
+    <t>gpx/trk/trkseg/trkpt/extensions/gpxtpx:TrackPointExtension/gpxtpx:cad</t>
+  </si>
+  <si>
+    <t>ma problem s tymto obalovakom parsne to ako field z XML obsahom, ak tam ale nie je expandne childy pekne</t>
+  </si>
+  <si>
+    <t>toto vyraba strava napriklad z SuuntoFITu</t>
+  </si>
+  <si>
+    <t>gps visualizer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Text of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GPS symbol name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. For interchange with other programs, use the exact spelling of the symbol as displayed on the GPS.  If the GPS abbreviates words, spell them out.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(classification) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of the waypoint.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -580,6 +827,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -653,9 +905,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -664,6 +913,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -980,42 +1232,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8909D83C-4036-AE48-BC90-C7A5A1198F41}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="43.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="60.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="60.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F2" s="7"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1024,22 +1281,25 @@
       <c r="D3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -1048,81 +1308,83 @@
       <c r="D4" s="14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -1130,31 +1392,31 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1164,31 +1426,31 @@
       <c r="C21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
@@ -1199,14 +1461,178 @@
         <v>27</v>
       </c>
     </row>
+    <row r="28" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{3E73D1B4-4031-1041-A5EB-3323235980FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1266,7 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93CBA28-8264-4D4A-9230-DC135B00FC23}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1280,22 +1706,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1321,19 +1747,19 @@
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">

</xml_diff>